<commit_message>
Error Fixed in time2
</commit_message>
<xml_diff>
--- a/event_schedule.xlsx
+++ b/event_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ace56c24a7d3a79/Desktop/success/TechUtsav/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC104830395979AA5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6AB6459-BC76-4D81-8AA9-11F5F25FD95F}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC104830395979AA5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E194827D-D811-4EE9-8412-DA4E194F0A61}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,14 +227,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -244,16 +241,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -262,42 +253,53 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -313,6 +315,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -581,15 +587,15 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.26953125" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.26953125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="17" style="19" customWidth="1"/>
     <col min="5" max="5" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -600,223 +606,223 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="21">
         <v>45952</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="5">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="23">
         <v>45954</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="10">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="23">
         <v>45954</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="23">
         <v>45954</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="23">
         <v>45954</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="23">
         <v>45954</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="23">
         <v>45955</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="10">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="23">
         <v>45955</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="23">
         <v>45955</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="10">
         <v>0.5</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="23">
         <v>45955</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>0.54166666666666663</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="22"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="18"/>
+      <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="23">
         <v>45955</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="5">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Updated the contact Page
</commit_message>
<xml_diff>
--- a/event_schedule.xlsx
+++ b/event_schedule.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ace56c24a7d3a79/Desktop/success/TechUtsav/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC104830395979AA5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E194827D-D811-4EE9-8412-DA4E194F0A61}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_F25DC773A252ABDACC104830395979AA5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2E12D12-7687-42E7-95FC-F3A90CD083F6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Coordinators" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Day</t>
   </si>
@@ -100,6 +101,36 @@
   </si>
   <si>
     <t>Final Dance and Singing Perfomance</t>
+  </si>
+  <si>
+    <t>Student Coordinator</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -109,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +151,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -227,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -300,6 +339,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.26953125" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -832,4 +877,123 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C3224E-B216-43BF-B73D-0F7B8EA8AA60}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.36328125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" style="27" customWidth="1"/>
+    <col min="3" max="16384" width="16.08984375" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="27">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>